<commit_message>
cg: updates some forms
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Congo/2024/cg_lf_pretas_2408_3_dbs.xlsx
+++ b/LF/PreTAS/Congo/2024/cg_lf_pretas_2408_3_dbs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\PreTAS\Congo\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6CE6BC-BA87-4370-88A0-3CCEF3808A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FAA8E4-FECD-473C-87EA-6861BE3C2B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -677,12 +677,6 @@
     <t>o_cluster_id2</t>
   </si>
   <si>
-    <t>if(${o_cluster_name1} = 'Autre', concat(o_cluster_name2), concat(o_cluster_name1))</t>
-  </si>
-  <si>
-    <t>if(${o_cluster_name1} = 'Autre', concat(o_cluster_id2), concat(o_cluster_id1))</t>
-  </si>
-  <si>
     <t>region</t>
   </si>
   <si>
@@ -720,6 +714,12 @@
   </si>
   <si>
     <t>concat(${o_recorderID}, '_', ${o_cluster_id}, '_', ${o_manual_code_id})</t>
+  </si>
+  <si>
+    <t>if(${o_cluster_name1} = 'Autre', concat(${o_cluster_name2}), concat(${o_cluster_name1}))</t>
+  </si>
+  <si>
+    <t>if(${o_cluster_name1} = 'Autre', concat(${o_cluster_id2}), concat(${o_cluster_id1}))</t>
   </si>
 </sst>
 </file>
@@ -1543,11 +1543,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1808,7 +1808,7 @@
       <c r="G9" s="50"/>
       <c r="H9" s="50"/>
       <c r="I9" s="50" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="J9" s="50" t="s">
         <v>16</v>
@@ -1820,7 +1820,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="9" customFormat="1" ht="31.5">
+    <row r="10" spans="1:15" s="9" customFormat="1" ht="47.25">
       <c r="A10" s="49" t="s">
         <v>17</v>
       </c>
@@ -1836,7 +1836,7 @@
       <c r="G10" s="50"/>
       <c r="H10" s="50"/>
       <c r="I10" s="50" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
       <c r="J10" s="50" t="s">
         <v>16</v>
@@ -2014,7 +2014,7 @@
       </c>
       <c r="H18" s="22"/>
       <c r="I18" s="24" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="J18" s="22" t="s">
         <v>16</v>
@@ -2562,7 +2562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A26" sqref="A26:XFD29"/>
     </sheetView>
@@ -2588,10 +2588,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>217</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>26</v>
@@ -2753,13 +2753,13 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="24" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D17" s="24"/>
     </row>
@@ -2768,16 +2768,16 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="24" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2788,13 +2788,13 @@
         <v>26</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2802,13 +2802,13 @@
         <v>26</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2816,13 +2816,13 @@
         <v>26</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2830,13 +2830,13 @@
         <v>26</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2850,7 +2850,7 @@
         <v>101</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2864,7 +2864,7 @@
         <v>102</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2878,40 +2878,40 @@
         <v>103</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="18" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B30" s="18">
         <v>101</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="18" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B31" s="18">
         <v>102</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="18" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B32" s="18">
         <v>103</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>